<commit_message>
syncing prior to aws migration
</commit_message>
<xml_diff>
--- a/SGBU_OCT_script.xlsx
+++ b/SGBU_OCT_script.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Tools\Python\Python Tools - Git Repos\SGBU_OCT_Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F4817E-2395-4DF2-A650-B70CE5D5D732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC6D5EC-29C1-42AA-A879-B60B22E624EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11205" yWindow="4440" windowWidth="26625" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="14430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Source</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>F:\Clients\SGBU\Tools\OCT\SGBU_OCT_output_13Feb23_test.csv</t>
+  </si>
+  <si>
+    <t>Fudge Factor</t>
   </si>
 </sst>
 </file>
@@ -569,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,7 +586,7 @@
     <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>25</v>
       </c>
@@ -605,8 +608,11 @@
       <c r="M1" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O1" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -629,25 +635,28 @@
       <c r="M2">
         <v>90</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E6" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added support for additional output with new conversion names and logic
</commit_message>
<xml_diff>
--- a/SGBU_OCT_script.xlsx
+++ b/SGBU_OCT_script.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Tools\Python\Python Tools - Git Repos\SGBU_OCT_Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC6D5EC-29C1-42AA-A879-B60B22E624EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E489A5-DDB8-4C6D-81B5-16B4AA84FED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="14430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="28740" windowHeight="14340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Source</t>
   </si>
@@ -146,6 +146,15 @@
   </si>
   <si>
     <t>Fudge Factor</t>
+  </si>
+  <si>
+    <t>19MGCdQZPN6ucU9prUqnhfxYmlGt2QO20w_IT6w3pVXA</t>
+  </si>
+  <si>
+    <t>F:\Tools\Python\credentials\wp_oct_api\custom-healer-187616-2e4a86fd3dc2.json</t>
+  </si>
+  <si>
+    <t>F:\Clients\SGBU\Tools\OCT\SGBU_OCT_output_22Mar24_conversion_test.csv</t>
   </si>
 </sst>
 </file>
@@ -252,9 +261,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -292,9 +301,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -327,26 +336,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -379,26 +371,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -575,7 +550,7 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,8 +616,16 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="C3" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="E3" s="4"/>
+      <c r="I3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>

</xml_diff>